<commit_message>
engi, docusaurus & new tigertrack structure
</commit_message>
<xml_diff>
--- a/SustSol/TimeTracking_2025.xlsx
+++ b/SustSol/TimeTracking_2025.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="170">
   <si>
     <t xml:space="preserve">SustSol Time Tracking</t>
   </si>
@@ -408,6 +408,9 @@
   </si>
   <si>
     <t xml:space="preserve">F&amp;E grant proposal WebViewer DICOM-WEB v0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Engi Call `casa-api` + Monday technical docs + docusaurus site generation</t>
   </si>
   <si>
     <t xml:space="preserve">Monday – rest of projects: epics &amp; tasks</t>
@@ -1699,13 +1702,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD1048576"/>
+  <dimension ref="A1:XFD219"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A165" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B175" activeCellId="0" sqref="B175"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A151" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A170" activeCellId="0" sqref="A170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="71"/>
@@ -5046,14 +5049,16 @@
     </row>
     <row r="169" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="n">
-        <v>45957</v>
+        <v>45959</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C169" s="16"/>
-      <c r="D169" s="16" t="s">
-        <v>130</v>
+      <c r="C169" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D169" s="16" t="n">
+        <v>1</v>
       </c>
       <c r="E169" s="16"/>
       <c r="F169" s="17"/>
@@ -5066,14 +5071,17 @@
       <c r="M169" s="18"/>
     </row>
     <row r="170" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A170" s="1" t="n">
+        <v>45960</v>
+      </c>
       <c r="B170" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C170" s="16"/>
+      <c r="D170" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="C170" s="16"/>
-      <c r="D170" s="16"/>
-      <c r="E170" s="16" t="s">
-        <v>130</v>
-      </c>
+      <c r="E170" s="16"/>
       <c r="F170" s="17"/>
       <c r="G170" s="17"/>
       <c r="H170" s="17"/>
@@ -5084,14 +5092,11 @@
       <c r="M170" s="18"/>
     </row>
     <row r="171" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B171" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="A171" s="0"/>
+      <c r="B171" s="0"/>
       <c r="C171" s="16"/>
       <c r="D171" s="16"/>
-      <c r="E171" s="16" t="s">
-        <v>130</v>
-      </c>
+      <c r="E171" s="16"/>
       <c r="F171" s="17"/>
       <c r="G171" s="17"/>
       <c r="H171" s="17"/>
@@ -5100,12 +5105,6 @@
       <c r="K171" s="18"/>
       <c r="L171" s="18"/>
       <c r="M171" s="18"/>
-      <c r="XEY171" s="21"/>
-      <c r="XEZ171" s="21"/>
-      <c r="XFA171" s="21"/>
-      <c r="XFB171" s="21"/>
-      <c r="XFC171" s="21"/>
-      <c r="XFD171" s="21"/>
     </row>
     <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C172" s="16"/>
@@ -5119,15 +5118,21 @@
       <c r="K172" s="18"/>
       <c r="L172" s="18"/>
       <c r="M172" s="18"/>
+      <c r="XEY172" s="21"/>
+      <c r="XEZ172" s="21"/>
+      <c r="XFA172" s="21"/>
+      <c r="XFB172" s="21"/>
+      <c r="XFC172" s="21"/>
+      <c r="XFD172" s="21"/>
     </row>
     <row r="173" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B173" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C173" s="16"/>
       <c r="D173" s="16"/>
       <c r="E173" s="16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F173" s="17"/>
       <c r="G173" s="17"/>
@@ -5139,9 +5144,14 @@
       <c r="M173" s="18"/>
     </row>
     <row r="174" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B174" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="C174" s="16"/>
       <c r="D174" s="16"/>
-      <c r="E174" s="16"/>
+      <c r="E174" s="16" t="s">
+        <v>131</v>
+      </c>
       <c r="F174" s="17"/>
       <c r="G174" s="17"/>
       <c r="H174" s="17"/>
@@ -5165,11 +5175,14 @@
       <c r="M175" s="18"/>
     </row>
     <row r="176" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A176" s="22"/>
-      <c r="B176" s="23"/>
-      <c r="C176" s="24"/>
-      <c r="D176" s="24"/>
-      <c r="E176" s="24"/>
+      <c r="B176" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C176" s="16"/>
+      <c r="D176" s="16"/>
+      <c r="E176" s="16" t="s">
+        <v>131</v>
+      </c>
       <c r="F176" s="17"/>
       <c r="G176" s="17"/>
       <c r="H176" s="17"/>
@@ -5180,11 +5193,9 @@
       <c r="M176" s="18"/>
     </row>
     <row r="177" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A177" s="22"/>
-      <c r="B177" s="23"/>
-      <c r="C177" s="24"/>
-      <c r="D177" s="24"/>
-      <c r="E177" s="24"/>
+      <c r="C177" s="16"/>
+      <c r="D177" s="16"/>
+      <c r="E177" s="16"/>
       <c r="F177" s="17"/>
       <c r="G177" s="17"/>
       <c r="H177" s="17"/>
@@ -5195,11 +5206,9 @@
       <c r="M177" s="18"/>
     </row>
     <row r="178" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A178" s="22"/>
-      <c r="B178" s="23"/>
-      <c r="C178" s="24"/>
-      <c r="D178" s="24"/>
-      <c r="E178" s="24"/>
+      <c r="C178" s="16"/>
+      <c r="D178" s="16"/>
+      <c r="E178" s="16"/>
       <c r="F178" s="17"/>
       <c r="G178" s="17"/>
       <c r="H178" s="17"/>
@@ -5255,9 +5264,11 @@
       <c r="M181" s="18"/>
     </row>
     <row r="182" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C182" s="16"/>
-      <c r="D182" s="16"/>
-      <c r="E182" s="16"/>
+      <c r="A182" s="22"/>
+      <c r="B182" s="23"/>
+      <c r="C182" s="24"/>
+      <c r="D182" s="24"/>
+      <c r="E182" s="24"/>
       <c r="F182" s="17"/>
       <c r="G182" s="17"/>
       <c r="H182" s="17"/>
@@ -5268,9 +5279,11 @@
       <c r="M182" s="18"/>
     </row>
     <row r="183" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C183" s="16"/>
-      <c r="D183" s="16"/>
-      <c r="E183" s="16"/>
+      <c r="A183" s="22"/>
+      <c r="B183" s="23"/>
+      <c r="C183" s="24"/>
+      <c r="D183" s="24"/>
+      <c r="E183" s="24"/>
       <c r="F183" s="17"/>
       <c r="G183" s="17"/>
       <c r="H183" s="17"/>
@@ -5281,10 +5294,11 @@
       <c r="M183" s="18"/>
     </row>
     <row r="184" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B184" s="21"/>
-      <c r="C184" s="16"/>
-      <c r="D184" s="16"/>
-      <c r="E184" s="16"/>
+      <c r="A184" s="22"/>
+      <c r="B184" s="23"/>
+      <c r="C184" s="24"/>
+      <c r="D184" s="24"/>
+      <c r="E184" s="24"/>
       <c r="F184" s="17"/>
       <c r="G184" s="17"/>
       <c r="H184" s="17"/>
@@ -5295,7 +5309,6 @@
       <c r="M184" s="18"/>
     </row>
     <row r="185" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B185" s="21"/>
       <c r="C185" s="16"/>
       <c r="D185" s="16"/>
       <c r="E185" s="16"/>
@@ -5309,7 +5322,6 @@
       <c r="M185" s="18"/>
     </row>
     <row r="186" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B186" s="15"/>
       <c r="C186" s="16"/>
       <c r="D186" s="16"/>
       <c r="E186" s="16"/>
@@ -5323,6 +5335,7 @@
       <c r="M186" s="18"/>
     </row>
     <row r="187" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B187" s="21"/>
       <c r="C187" s="16"/>
       <c r="D187" s="16"/>
       <c r="E187" s="16"/>
@@ -5336,6 +5349,7 @@
       <c r="M187" s="18"/>
     </row>
     <row r="188" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B188" s="21"/>
       <c r="C188" s="16"/>
       <c r="D188" s="16"/>
       <c r="E188" s="16"/>
@@ -5349,206 +5363,189 @@
       <c r="M188" s="18"/>
     </row>
     <row r="189" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A189" s="25" t="s">
-        <v>134</v>
-      </c>
       <c r="B189" s="15"/>
-      <c r="C189" s="26" t="n">
-        <f aca="false">SUM(C4:C188)</f>
-        <v>48</v>
-      </c>
-      <c r="D189" s="26" t="n">
-        <f aca="false">SUM(D4:D188)</f>
-        <v>72</v>
-      </c>
-      <c r="E189" s="26" t="n">
-        <f aca="false">SUM(E4:E188)</f>
+      <c r="C189" s="16"/>
+      <c r="D189" s="16"/>
+      <c r="E189" s="16"/>
+      <c r="F189" s="17"/>
+      <c r="G189" s="17"/>
+      <c r="H189" s="17"/>
+      <c r="I189" s="17"/>
+      <c r="J189" s="18"/>
+      <c r="K189" s="18"/>
+      <c r="L189" s="18"/>
+      <c r="M189" s="18"/>
+    </row>
+    <row r="190" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C190" s="16"/>
+      <c r="D190" s="16"/>
+      <c r="E190" s="16"/>
+      <c r="F190" s="17"/>
+      <c r="G190" s="17"/>
+      <c r="H190" s="17"/>
+      <c r="I190" s="17"/>
+      <c r="J190" s="18"/>
+      <c r="K190" s="18"/>
+      <c r="L190" s="18"/>
+      <c r="M190" s="18"/>
+    </row>
+    <row r="191" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C191" s="16"/>
+      <c r="D191" s="16"/>
+      <c r="E191" s="16"/>
+      <c r="F191" s="17"/>
+      <c r="G191" s="17"/>
+      <c r="H191" s="17"/>
+      <c r="I191" s="17"/>
+      <c r="J191" s="18"/>
+      <c r="K191" s="18"/>
+      <c r="L191" s="18"/>
+      <c r="M191" s="18"/>
+    </row>
+    <row r="192" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A192" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="B192" s="15"/>
+      <c r="C192" s="26" t="n">
+        <f aca="false">SUM(C4:C191)</f>
+        <v>49</v>
+      </c>
+      <c r="D192" s="26" t="n">
+        <f aca="false">SUM(D4:D191)</f>
+        <v>73</v>
+      </c>
+      <c r="E192" s="26" t="n">
+        <f aca="false">SUM(E4:E191)</f>
         <v>146</v>
       </c>
-      <c r="F189" s="27" t="n">
-        <f aca="false">SUM(F4:F188)</f>
+      <c r="F192" s="27" t="n">
+        <f aca="false">SUM(F4:F191)</f>
         <v>8.5</v>
       </c>
-      <c r="G189" s="27" t="n">
-        <f aca="false">SUM(G4:G188)</f>
+      <c r="G192" s="27" t="n">
+        <f aca="false">SUM(G4:G191)</f>
         <v>85</v>
       </c>
-      <c r="H189" s="27" t="n">
-        <f aca="false">SUM(H4:H188)</f>
+      <c r="H192" s="27" t="n">
+        <f aca="false">SUM(H4:H191)</f>
         <v>1</v>
       </c>
-      <c r="I189" s="27" t="n">
-        <f aca="false">SUM(I4:I188)</f>
+      <c r="I192" s="27" t="n">
+        <f aca="false">SUM(I4:I191)</f>
         <v>0</v>
       </c>
-      <c r="J189" s="27" t="n">
-        <f aca="false">SUM(J4:J188)</f>
+      <c r="J192" s="27" t="n">
+        <f aca="false">SUM(J4:J191)</f>
         <v>51.5</v>
       </c>
-      <c r="K189" s="27" t="n">
-        <f aca="false">SUM(K4:K188)</f>
+      <c r="K192" s="27" t="n">
+        <f aca="false">SUM(K4:K191)</f>
         <v>0</v>
       </c>
-      <c r="L189" s="27" t="n">
-        <f aca="false">SUM(L4:L188)</f>
+      <c r="L192" s="27" t="n">
+        <f aca="false">SUM(L4:L191)</f>
         <v>0</v>
       </c>
-      <c r="M189" s="27" t="n">
-        <f aca="false">SUM(M4:M188)</f>
+      <c r="M192" s="27" t="n">
+        <f aca="false">SUM(M4:M191)</f>
         <v>0</v>
       </c>
-      <c r="N189" s="15"/>
-      <c r="O189" s="15"/>
-      <c r="P189" s="15"/>
-      <c r="Q189" s="15"/>
-      <c r="R189" s="15"/>
-      <c r="S189" s="15"/>
-      <c r="T189" s="15"/>
-      <c r="U189" s="15"/>
-      <c r="V189" s="15"/>
-      <c r="W189" s="15"/>
-      <c r="X189" s="15"/>
-      <c r="Y189" s="15"/>
-      <c r="Z189" s="15"/>
-      <c r="AA189" s="15"/>
-      <c r="AB189" s="15"/>
-      <c r="AC189" s="15"/>
-      <c r="AD189" s="15"/>
-      <c r="AE189" s="15"/>
-    </row>
-    <row r="190" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B190" s="15"/>
-      <c r="C190" s="28"/>
-      <c r="D190" s="28"/>
-      <c r="E190" s="28"/>
-      <c r="F190" s="28"/>
-      <c r="G190" s="28"/>
-      <c r="H190" s="28"/>
-      <c r="I190" s="28"/>
-      <c r="J190" s="28"/>
-      <c r="K190" s="28"/>
-      <c r="L190" s="28"/>
-      <c r="M190" s="28"/>
-    </row>
-    <row r="191" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B191" s="15"/>
-      <c r="D191" s="29"/>
-      <c r="E191" s="29"/>
-      <c r="F191" s="28"/>
-      <c r="H191" s="30"/>
-      <c r="I191" s="30"/>
-      <c r="J191" s="28"/>
-      <c r="K191" s="28"/>
-      <c r="L191" s="31"/>
-      <c r="M191" s="31"/>
-    </row>
-    <row r="192" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B192" s="15"/>
-      <c r="D192" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="E192" s="29" t="n">
-        <f aca="false">SUM(C189:E189)</f>
-        <v>266</v>
-      </c>
-      <c r="F192" s="28"/>
-      <c r="H192" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="I192" s="30" t="n">
-        <f aca="false">SUM(F189:I189)</f>
-        <v>94.5</v>
-      </c>
-      <c r="J192" s="28"/>
-      <c r="K192" s="28"/>
-      <c r="L192" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="M192" s="31" t="n">
-        <f aca="false">SUM(J189:M189)</f>
-        <v>51.5</v>
-      </c>
-    </row>
-    <row r="193" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N192" s="15"/>
+      <c r="O192" s="15"/>
+      <c r="P192" s="15"/>
+      <c r="Q192" s="15"/>
+      <c r="R192" s="15"/>
+      <c r="S192" s="15"/>
+      <c r="T192" s="15"/>
+      <c r="U192" s="15"/>
+      <c r="V192" s="15"/>
+      <c r="W192" s="15"/>
+      <c r="X192" s="15"/>
+      <c r="Y192" s="15"/>
+      <c r="Z192" s="15"/>
+      <c r="AA192" s="15"/>
+      <c r="AB192" s="15"/>
+      <c r="AC192" s="15"/>
+      <c r="AD192" s="15"/>
+      <c r="AE192" s="15"/>
+    </row>
+    <row r="193" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B193" s="15"/>
-      <c r="D193" s="29"/>
-      <c r="E193" s="29"/>
+      <c r="C193" s="28"/>
+      <c r="D193" s="28"/>
+      <c r="E193" s="28"/>
       <c r="F193" s="28"/>
-      <c r="H193" s="30"/>
-      <c r="I193" s="30"/>
+      <c r="G193" s="28"/>
+      <c r="H193" s="28"/>
+      <c r="I193" s="28"/>
       <c r="J193" s="28"/>
       <c r="K193" s="28"/>
-      <c r="L193" s="31"/>
-      <c r="M193" s="31"/>
+      <c r="L193" s="28"/>
+      <c r="M193" s="28"/>
     </row>
     <row r="194" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B194" s="15"/>
-      <c r="D194" s="35"/>
-      <c r="E194" s="35"/>
+      <c r="D194" s="29"/>
+      <c r="E194" s="29"/>
       <c r="F194" s="28"/>
-      <c r="H194" s="35"/>
-      <c r="I194" s="35"/>
+      <c r="H194" s="30"/>
+      <c r="I194" s="30"/>
       <c r="J194" s="28"/>
       <c r="K194" s="28"/>
-      <c r="L194" s="36"/>
-      <c r="M194" s="36"/>
-    </row>
-    <row r="195" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L194" s="31"/>
+      <c r="M194" s="31"/>
+    </row>
+    <row r="195" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B195" s="15"/>
-      <c r="D195" s="37"/>
-      <c r="E195" s="38"/>
-      <c r="H195" s="39"/>
-      <c r="I195" s="40"/>
-      <c r="L195" s="41"/>
-      <c r="M195" s="42"/>
-    </row>
-    <row r="196" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D195" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E195" s="29" t="n">
+        <f aca="false">SUM(C192:E192)</f>
+        <v>268</v>
+      </c>
+      <c r="F195" s="28"/>
+      <c r="H195" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="I195" s="30" t="n">
+        <f aca="false">SUM(F192:I192)</f>
+        <v>94.5</v>
+      </c>
+      <c r="J195" s="28"/>
+      <c r="K195" s="28"/>
+      <c r="L195" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="M195" s="31" t="n">
+        <f aca="false">SUM(J192:M192)</f>
+        <v>51.5</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B196" s="15"/>
-      <c r="D196" s="43" t="n">
-        <v>2025</v>
-      </c>
-      <c r="E196" s="44" t="n">
-        <f aca="false">SUM(C4:E188)</f>
-        <v>266</v>
-      </c>
-      <c r="H196" s="45" t="n">
-        <v>2025</v>
-      </c>
-      <c r="I196" s="46" t="n">
-        <f aca="false">SUM(F4:I188)</f>
-        <v>94.5</v>
-      </c>
-      <c r="L196" s="47" t="n">
-        <v>2025</v>
-      </c>
-      <c r="M196" s="48" t="n">
-        <f aca="false">SUM(J4:M188)</f>
-        <v>51.5</v>
-      </c>
-    </row>
-    <row r="197" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D196" s="29"/>
+      <c r="E196" s="29"/>
+      <c r="F196" s="28"/>
+      <c r="H196" s="30"/>
+      <c r="I196" s="30"/>
+      <c r="J196" s="28"/>
+      <c r="K196" s="28"/>
+      <c r="L196" s="31"/>
+      <c r="M196" s="31"/>
+    </row>
+    <row r="197" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B197" s="15"/>
-      <c r="D197" s="49" t="s">
-        <v>135</v>
-      </c>
-      <c r="E197" s="44" t="n">
-        <f aca="false">SUM(C155:E188)</f>
-        <v>27</v>
-      </c>
-      <c r="H197" s="50" t="s">
-        <v>135</v>
-      </c>
-      <c r="I197" s="46" t="n">
-        <f aca="false">SUM(F155:I188)</f>
-        <v>2</v>
-      </c>
-      <c r="L197" s="51" t="s">
-        <v>135</v>
-      </c>
-      <c r="M197" s="48" t="n">
-        <f aca="false">SUM(J155:M188)</f>
-        <v>0</v>
-      </c>
+      <c r="D197" s="35"/>
+      <c r="E197" s="35"/>
+      <c r="F197" s="28"/>
+      <c r="H197" s="35"/>
+      <c r="I197" s="35"/>
+      <c r="J197" s="28"/>
+      <c r="K197" s="28"/>
+      <c r="L197" s="36"/>
+      <c r="M197" s="36"/>
     </row>
     <row r="198" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B198" s="15"/>
@@ -5556,132 +5553,187 @@
       <c r="E198" s="38"/>
       <c r="H198" s="39"/>
       <c r="I198" s="40"/>
-      <c r="K198" s="52"/>
       <c r="L198" s="41"/>
       <c r="M198" s="42"/>
     </row>
-    <row r="199" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B199" s="15"/>
-      <c r="E199" s="28"/>
-      <c r="K199" s="52"/>
-      <c r="M199" s="28"/>
-    </row>
-    <row r="200" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D199" s="43" t="n">
+        <v>2025</v>
+      </c>
+      <c r="E199" s="44" t="n">
+        <f aca="false">SUM(C4:E191)</f>
+        <v>268</v>
+      </c>
+      <c r="H199" s="45" t="n">
+        <v>2025</v>
+      </c>
+      <c r="I199" s="46" t="n">
+        <f aca="false">SUM(F4:I191)</f>
+        <v>94.5</v>
+      </c>
+      <c r="L199" s="47" t="n">
+        <v>2025</v>
+      </c>
+      <c r="M199" s="48" t="n">
+        <f aca="false">SUM(J4:M191)</f>
+        <v>51.5</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B200" s="15"/>
-      <c r="E200" s="28"/>
-      <c r="K200" s="53"/>
-      <c r="L200" s="54"/>
-      <c r="M200" s="55"/>
-    </row>
-    <row r="201" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D200" s="49" t="s">
+        <v>136</v>
+      </c>
+      <c r="E200" s="44" t="n">
+        <f aca="false">SUM(C155:E191)</f>
+        <v>29</v>
+      </c>
+      <c r="H200" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="I200" s="46" t="n">
+        <f aca="false">SUM(F155:I191)</f>
+        <v>2</v>
+      </c>
+      <c r="L200" s="51" t="s">
+        <v>136</v>
+      </c>
+      <c r="M200" s="48" t="n">
+        <f aca="false">SUM(J155:M191)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B201" s="15"/>
-      <c r="E201" s="28"/>
-      <c r="K201" s="53" t="s">
-        <v>136</v>
-      </c>
-      <c r="L201" s="56"/>
-      <c r="M201" s="57" t="n">
-        <f aca="false">SUM(C4:M188)</f>
-        <v>412</v>
-      </c>
-    </row>
-    <row r="202" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K202" s="53" t="s">
-        <v>135</v>
-      </c>
-      <c r="L202" s="58"/>
-      <c r="M202" s="57" t="n">
-        <f aca="false">E197+I197+M197</f>
-        <v>29</v>
-      </c>
+      <c r="D201" s="37"/>
+      <c r="E201" s="38"/>
+      <c r="H201" s="39"/>
+      <c r="I201" s="40"/>
+      <c r="K201" s="52"/>
+      <c r="L201" s="41"/>
+      <c r="M201" s="42"/>
+    </row>
+    <row r="202" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B202" s="15"/>
+      <c r="E202" s="28"/>
+      <c r="K202" s="52"/>
+      <c r="M202" s="28"/>
     </row>
     <row r="203" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K203" s="54"/>
+      <c r="B203" s="15"/>
+      <c r="E203" s="28"/>
+      <c r="K203" s="53"/>
       <c r="L203" s="54"/>
       <c r="M203" s="55"/>
     </row>
-    <row r="204" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C204" s="28"/>
-      <c r="K204" s="59" t="s">
+    <row r="204" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B204" s="15"/>
+      <c r="E204" s="28"/>
+      <c r="K204" s="53" t="s">
         <v>137</v>
       </c>
-      <c r="M204" s="2" t="n">
+      <c r="L204" s="56"/>
+      <c r="M204" s="57" t="n">
+        <f aca="false">SUM(C4:M191)</f>
+        <v>414</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K205" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="L205" s="58"/>
+      <c r="M205" s="57" t="n">
+        <f aca="false">E200+I200+M200</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K206" s="54"/>
+      <c r="L206" s="54"/>
+      <c r="M206" s="55"/>
+    </row>
+    <row r="207" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C207" s="28"/>
+      <c r="K207" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="M207" s="2" t="n">
         <v>200</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B205" s="60" t="s">
-        <v>138</v>
-      </c>
-      <c r="C205" s="28"/>
-      <c r="K205" s="2" t="s">
+    <row r="208" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B208" s="60" t="s">
         <v>139</v>
       </c>
-      <c r="M205" s="2" t="n">
-        <f aca="false">M204-M202</f>
-        <v>171</v>
-      </c>
-    </row>
-    <row r="206" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C206" s="28"/>
-      <c r="K206" s="2" t="s">
+      <c r="C208" s="28"/>
+      <c r="K208" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="M206" s="2" t="n">
-        <f aca="false">M205/8</f>
-        <v>21.375</v>
-      </c>
-    </row>
-    <row r="207" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B207" s="2" t="s">
+      <c r="M208" s="2" t="n">
+        <f aca="false">M207-M205</f>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C209" s="28"/>
+      <c r="K209" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C207" s="28"/>
-    </row>
-    <row r="208" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B208" s="2" t="s">
+      <c r="M209" s="2" t="n">
+        <f aca="false">M208/8</f>
+        <v>21.125</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B210" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C208" s="28"/>
-    </row>
-    <row r="209" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B209" s="2" t="s">
+      <c r="C210" s="28"/>
+    </row>
+    <row r="211" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B211" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C209" s="61"/>
-    </row>
-    <row r="210" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B210" s="2" t="s">
+      <c r="C211" s="28"/>
+    </row>
+    <row r="212" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B212" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="212" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B212" s="15" t="s">
+      <c r="C212" s="61"/>
+    </row>
+    <row r="213" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B213" s="2" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="213" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B213" s="15" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="214" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B214" s="15" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B215" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B216" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B217" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B218" s="15" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="219" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B219" s="15" t="s">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C2:E2"/>
@@ -5709,7 +5761,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="62" width="3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="62" width="18.16"/>
@@ -5740,99 +5792,99 @@
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="63"/>
       <c r="B2" s="64" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C2" s="65"/>
       <c r="D2" s="63"/>
       <c r="E2" s="66" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F2" s="67"/>
       <c r="G2" s="63"/>
       <c r="H2" s="66" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I2" s="67"/>
       <c r="J2" s="63"/>
       <c r="K2" s="66" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="L2" s="67"/>
       <c r="M2" s="63"/>
       <c r="N2" s="66" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O2" s="68"/>
       <c r="P2" s="63"/>
       <c r="Q2" s="66" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="R2" s="67"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="63"/>
       <c r="B3" s="69" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C3" s="65" t="n">
-        <f aca="false">SUM(Tasks_23_24!C341:E341)</f>
+        <f aca="false">SUM(Tasks_23_24!C344:E344)</f>
         <v>0</v>
       </c>
       <c r="D3" s="63"/>
       <c r="E3" s="70" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F3" s="71" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G3" s="63"/>
       <c r="H3" s="70" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I3" s="71" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="J3" s="63"/>
       <c r="K3" s="70" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L3" s="71" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M3" s="63"/>
       <c r="N3" s="70" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="O3" s="71" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="P3" s="63"/>
       <c r="Q3" s="70" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="R3" s="71" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="63"/>
       <c r="B4" s="72" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C4" s="73" t="n">
         <v>100</v>
       </c>
       <c r="D4" s="63"/>
       <c r="E4" s="68" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F4" s="74" t="e">
-        <f aca="false">SUM(Tasks_23_24!F511:G511)+#REF!*228/496</f>
+        <f aca="false">SUM(Tasks_23_24!F514:G514)+#REF!*228/496</f>
         <v>#REF!</v>
       </c>
       <c r="G4" s="63"/>
       <c r="H4" s="68" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I4" s="74" t="e">
         <f aca="false">#REF!+#REF!*80/496</f>
@@ -5840,15 +5892,15 @@
       </c>
       <c r="J4" s="63"/>
       <c r="K4" s="68" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="L4" s="74" t="e">
-        <f aca="false">Tasks_23_24!H511+#REF!*36/496</f>
+        <f aca="false">Tasks_23_24!H514+#REF!*36/496</f>
         <v>#REF!</v>
       </c>
       <c r="M4" s="63"/>
       <c r="N4" s="68" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="O4" s="74" t="e">
         <f aca="false">#REF!+#REF!*24/496</f>
@@ -5856,17 +5908,17 @@
       </c>
       <c r="P4" s="63"/>
       <c r="Q4" s="68" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="R4" s="74" t="e">
-        <f aca="false">Tasks_23_24!I511+#REF!*128/496</f>
+        <f aca="false">Tasks_23_24!I514+#REF!*128/496</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="63"/>
       <c r="B5" s="75" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C5" s="76" t="n">
         <f aca="false">C3*C4</f>
@@ -5874,35 +5926,35 @@
       </c>
       <c r="D5" s="63"/>
       <c r="E5" s="77" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F5" s="78" t="n">
         <v>100</v>
       </c>
       <c r="G5" s="63"/>
       <c r="H5" s="77" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I5" s="78" t="n">
         <v>100</v>
       </c>
       <c r="J5" s="63"/>
       <c r="K5" s="77" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L5" s="78" t="n">
         <v>100</v>
       </c>
       <c r="M5" s="63"/>
       <c r="N5" s="77" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="O5" s="78" t="n">
         <v>100</v>
       </c>
       <c r="P5" s="63"/>
       <c r="Q5" s="77" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R5" s="78" t="n">
         <v>100</v>
@@ -5911,7 +5963,7 @@
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="63"/>
       <c r="B6" s="72" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C6" s="79" t="n">
         <f aca="false">C5*0.2</f>
@@ -5919,7 +5971,7 @@
       </c>
       <c r="D6" s="63"/>
       <c r="E6" s="80" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F6" s="81" t="e">
         <f aca="false">F4*F5</f>
@@ -5927,7 +5979,7 @@
       </c>
       <c r="G6" s="63"/>
       <c r="H6" s="80" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I6" s="81" t="e">
         <f aca="false">I4*I5</f>
@@ -5935,7 +5987,7 @@
       </c>
       <c r="J6" s="63"/>
       <c r="K6" s="80" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="L6" s="81" t="e">
         <f aca="false">L4*L5</f>
@@ -5943,7 +5995,7 @@
       </c>
       <c r="M6" s="63"/>
       <c r="N6" s="80" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="O6" s="81" t="e">
         <f aca="false">O4*O5</f>
@@ -5951,7 +6003,7 @@
       </c>
       <c r="P6" s="63"/>
       <c r="Q6" s="80" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="R6" s="81" t="e">
         <f aca="false">R4*R5</f>
@@ -5961,7 +6013,7 @@
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="63"/>
       <c r="B7" s="82" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C7" s="83" t="n">
         <f aca="false">C5+C6</f>
@@ -5969,7 +6021,7 @@
       </c>
       <c r="D7" s="63"/>
       <c r="E7" s="77" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F7" s="74" t="e">
         <f aca="false">F6*0.2</f>
@@ -5977,7 +6029,7 @@
       </c>
       <c r="G7" s="63"/>
       <c r="H7" s="77" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I7" s="74" t="e">
         <f aca="false">I6*0.2</f>
@@ -5985,7 +6037,7 @@
       </c>
       <c r="J7" s="63"/>
       <c r="K7" s="77" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="L7" s="74" t="e">
         <f aca="false">L6*0.2</f>
@@ -5993,7 +6045,7 @@
       </c>
       <c r="M7" s="63"/>
       <c r="N7" s="77" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="O7" s="74" t="e">
         <f aca="false">O6*0.2</f>
@@ -6001,7 +6053,7 @@
       </c>
       <c r="P7" s="63"/>
       <c r="Q7" s="77" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="R7" s="74" t="e">
         <f aca="false">R6*0.2</f>
@@ -6010,7 +6062,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E8" s="82" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F8" s="83" t="e">
         <f aca="false">F6+F7</f>
@@ -6018,7 +6070,7 @@
       </c>
       <c r="G8" s="63"/>
       <c r="H8" s="82" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I8" s="83" t="e">
         <f aca="false">I6+I7</f>
@@ -6026,7 +6078,7 @@
       </c>
       <c r="J8" s="63"/>
       <c r="K8" s="82" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="L8" s="83" t="e">
         <f aca="false">L6+L7</f>
@@ -6034,7 +6086,7 @@
       </c>
       <c r="M8" s="63"/>
       <c r="N8" s="82" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O8" s="83" t="e">
         <f aca="false">O6+O7</f>
@@ -6042,7 +6094,7 @@
       </c>
       <c r="P8" s="63"/>
       <c r="Q8" s="82" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="R8" s="83" t="e">
         <f aca="false">R6+R7</f>
@@ -6054,15 +6106,15 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E10" s="70" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F10" s="71" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E11" s="62" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F11" s="84" t="e">
         <f aca="false">F4+I4+L4+R4+O4</f>
@@ -6071,7 +6123,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E12" s="82" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F12" s="83" t="e">
         <f aca="false">F6+I6+L6+R6+O6</f>
@@ -6081,7 +6133,7 @@
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="63"/>
       <c r="B13" s="85" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C13" s="86" t="e">
         <f aca="false">C7+F12</f>

</xml_diff>